<commit_message>
Cleaned up unused/old code
</commit_message>
<xml_diff>
--- a/data/250616_HTE.xlsx
+++ b/data/250616_HTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Documents/Water_Splitting/Projects/HTE_Photocatalysis/HTE_Streamlit_App/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7675640B-E1B0-2747-B212-F384D78A9F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E975A23-756F-1B4D-A1F8-C137AAEFE898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1780" windowWidth="28800" windowHeight="13300" xr2:uid="{1823FD07-5DF0-4D9D-8668-30FF8962221A}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>Experiment</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>MRG-059-ZN-12B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -465,13 +468,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D11C39-576A-41CB-989F-A3A489A4D2A6}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2589,20 +2591,9 @@
         <v>8.8299999999999993E-3</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="3">
-        <f>C63*1000000</f>
-        <v>100</v>
-      </c>
-      <c r="E70" s="3">
-        <f>C5*1000000</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E72" s="3">
-        <f>D59*1000000</f>
-        <v>6000</v>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>